<commit_message>
Demo dashbaord log 1
</commit_message>
<xml_diff>
--- a/table-1.xlsx
+++ b/table-1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,45 +464,56 @@
           <t>topic_contribution</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>aspect_based_sentiment</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>68</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>I bought a phone, but they didn’t inform me of all the hidden fees.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-11-12</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>The staff were incredibly helpful and patient, helping me find the perfect phone!</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2024-11-01</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
-      </c>
       <c r="F2" t="n">
-        <v>0.6150000095367432</v>
+        <v>0.6541000008583069</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - buy : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I had a great experience purchasing my phone here, the process was smooth and quick.</t>
+          <t>I received excellent advice from the sales team, they really know their products.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -511,62 +522,82 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6103000044822693</v>
+        <v>0.6529999971389771</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - know, receive : Positive
+● store - know : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Their selection of phones is amazing, and the prices are very competitive!</t>
+          <t>The store was messy and understaffed.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7455000281333923</v>
+        <v>0.6488999724388123</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - understaffed : Neutral
+● store - messy : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I appreciate how the staff walked me through setting up my new device.</t>
+          <t>The store was chaotic, with long lines and unhelpful staff.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-16</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7651000022888184</v>
+        <v>0.6322000026702881</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● long lines - lines : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -594,71 +625,89 @@
       <c r="F6" t="n">
         <v>0.6252999901771545</v>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● question - answer : Neutral
+</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>They offer amazing deals on phones, I couldn’t resist upgrading.</t>
+          <t>I felt pressured to buy accessories I didn’t need.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4323999881744385</v>
+        <v>0.6230999827384949</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - feel : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The technician fixed my phone’s issue faster than I expected. Highly recommend!</t>
+          <t>I felt overcharged for a simple screen repair.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-17</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7358999848365784</v>
+        <v>0.6230999827384949</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - feel : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fantastic experience, the staff really know their stuff!</t>
+          <t>Their warranty plan is worth every penny, such a relief!</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-06</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -667,76 +716,95 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5684999823570251</v>
+        <v>0.6154999732971191</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● plan - worth : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>I found the perfect phone case here, and the variety was impressive.</t>
+          <t>Best phone store in town, hands down!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7077999711036682</v>
+        <v>0.6021999716758728</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - hand : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Upgrading my phone was a breeze thanks to their professional service.</t>
+          <t>They upsold me on a phone plan I didn’t need, very deceptive.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.571399986743927</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - upsold : Neutral
+● store - upsold : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Staff was knowledgeable and made sure I knew everything about my new phone.</t>
+          <t>This is my go-to store for any phone issues, always reliable.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-08</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -745,24 +813,30 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6011000275611877</v>
+        <v>0.5602999925613403</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - reliable : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Prices were reasonable and the staff very courteous!</t>
+          <t>Very professional and friendly service, I’m super satisfied!</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -774,47 +848,59 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5030999779701233</v>
+        <v>0.5587000250816345</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - m : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Very happy with my purchase, the staff really went the extra mile.</t>
+          <t>Great variety of phones, and the staff was very patient with my questions.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6010000109672546</v>
+        <v>0.5346000194549561</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● variety - patient : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Excellent service! They helped me find exactly what I was looking for.</t>
+          <t>They resolved my issue very quickly and professionally.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -823,102 +909,129 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0.7067000269889832</v>
+        <v>0.5146999955177307</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - resolve : Positive
+● store - resolve : Positive
+● store - resolve : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Great deals on accessories, and the staff was super friendly!</t>
+          <t>They helped me choose a phone within my budget, which I really appreciated.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024-11-01</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7020000219345093</v>
+        <v>0.5077000260353088</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - help, choose : Neutral
+● store - help, choose : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>I love this store! Always a smooth experience buying or fixing my phone.</t>
+          <t>Prices were reasonable and the staff very courteous!</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7172999978065491</v>
+        <v>0.5030999779701233</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● price - reasonable : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>I got a really good trade-in deal on my old phone.</t>
+          <t>I had to wait over an hour to be helped, and the staff wasn’t apologetic at all.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5996000170707703</v>
+        <v>0.4941000044345856</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - apologetic : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Their repair services are quick and reliable.</t>
+          <t>The staff was unprofessional and seemed like they didn’t want to be there.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -927,128 +1040,160 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5436999797821045</v>
+        <v>0.4939999878406525</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - unprofessional : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The staff was extremely helpful in setting up my phone and transferring all my data.</t>
+          <t>I’m a loyal customer because their customer service is always outstanding.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>0.4796999990940094</v>
+        <v>0.4923000037670135</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - outstanding : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Very professional and friendly service, I’m super satisfied!</t>
+          <t>Customer service was extremely slow, they need to hire more staff.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5587000250816345</v>
+        <v>0.4921999871730804</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - slow : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Great variety of phones, and the staff was very patient with my questions.</t>
+          <t>They offer amazing deals on phones, I couldn’t resist upgrading.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E22" t="n">
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5346000194549561</v>
+        <v>0.4323999881744385</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - resist, offer : Positive
+● staff - resist : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>The process was super simple, and I’m thrilled with my new phone.</t>
+          <t>I always leave this store feeling like I made the right purchase.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6927000284194946</v>
+        <v>0.7670999765396118</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - leave : Neutral
+● staff - make : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>They helped me choose a phone within my budget, which I really appreciated.</t>
+          <t>Staff seemed untrained and gave me incorrect information about the phone plan.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-12</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1057,24 +1202,30 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5077000260353088</v>
+        <v>0.7663000226020813</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone plan - give : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>My phone was fixed in less than 30 minutes, such fast service!</t>
+          <t>I appreciate how the staff walked me through setting up my new device.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1083,24 +1234,31 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>0.7124999761581421</v>
+        <v>0.7651000022888184</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - appreciate, walk : Neutral
+● staff - appreciate, walk : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>I’m a loyal customer because their customer service is always outstanding.</t>
+          <t>I’ve been to many phone stores, but this one by far provides the best service.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2024-11-03</t>
+          <t>2024-11-05</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1109,45 +1267,57 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" t="n">
-        <v>0.4923000037670135</v>
+        <v>0.7523000240325928</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● one - provide : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Best phone store in town, hands down!</t>
+          <t>The store layout is easy to navigate and staff are always ready to help.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-05</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>0.6021999716758728</v>
+        <v>0.7512000203132629</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - ready : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>The staff made sure I was completely comfortable with my purchase.</t>
+          <t>This store has a fantastic warranty service!</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1157,80 +1327,98 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E28" t="n">
         <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6974999904632568</v>
+        <v>0.7488999962806702</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - have : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>I found exactly what I needed, and they helped me get a great deal.</t>
+          <t>I had to return a faulty phone twice before they finally gave me a refund.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>0.7093999981880188</v>
+        <v>0.7469000220298767</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - have, return : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>This store has a fantastic warranty service!</t>
+          <t>They refused to honor the promotion I came in for, very misleading.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E30" t="n">
         <v>2</v>
       </c>
       <c r="F30" t="n">
-        <v>0.7488999962806702</v>
+        <v>0.738099992275238</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - refuse, honor : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The staff was very informative, I learned a lot about phone features I didn’t know about.</t>
+          <t>Service was quick and efficient, I was in and out within 15 minutes!</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-07</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1242,73 +1430,94 @@
         <v>2</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6934000253677368</v>
+        <v>0.7379000186920166</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - quick : Positive
+● service - efficient : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Excellent store for buying phone accessories, so much variety!</t>
+          <t>Best pricing for phone plans, they helped me save a lot!</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-05</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>0.7236999869346619</v>
+        <v>0.7348999977111816</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - help, save : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The phone I bought here is working perfectly, couldn’t be happier.</t>
+          <t>They even helped me transfer all my contacts and data without extra charge.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-08</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E33" t="n">
         <v>2</v>
       </c>
       <c r="F33" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.7339000105857849</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - help, transfer : Neutral
+● store - help, transfer : Neutral
+● store - help, transfer : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>They were super quick in setting up my phone, I was out of there in no time.</t>
+          <t>Highly recommend this store if you’re looking for good deals on phones!</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2024-11-04</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1320,16 +1529,22 @@
         <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6705999970436096</v>
+        <v>0.7299000024795532</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - look : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Always come here for upgrades, they never disappoint!</t>
+          <t>Excellent store for buying phone accessories, so much variety!</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1346,21 +1561,27 @@
         <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.7236999869346619</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - excellent : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The store layout is easy to navigate and staff are always ready to help.</t>
+          <t>They offer fantastic promotions and discounts!</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2024-11-05</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1372,151 +1593,189 @@
         <v>2</v>
       </c>
       <c r="F36" t="n">
-        <v>0.7512000203132629</v>
+        <v>0.7225000262260437</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - offer : Positive
+● store - offer : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Best pricing for phone plans, they helped me save a lot!</t>
+          <t>Customer service is poor, no one seemed interested in helping me.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2024-11-05</t>
+          <t>2024-11-11</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E37" t="n">
         <v>2</v>
       </c>
       <c r="F37" t="n">
-        <v>0.7348999977111816</v>
+        <v>0.7172999978065491</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - poor : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>I’ve been to many phone stores, but this one by far provides the best service.</t>
+          <t>The staff was rude and unhelpful, I’m never coming back.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2024-11-05</t>
+          <t>2024-11-11</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E38" t="n">
         <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>0.7523000240325928</v>
+        <v>0.7110999822616577</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - rude : Negative
+● staff - unhelpful : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Customer service here is top-notch, they always resolve my issues quickly.</t>
+          <t>Their return policy is awful, I couldn’t exchange my phone despite its defects.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2024-11-05</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E39" t="n">
         <v>2</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7006000280380249</v>
+        <v>0.7081999778747559</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● policy - awful : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>I always recommend this store to friends and family, they never fail to impress.</t>
+          <t>They kept trying to sell me more expensive phones when I clearly stated my budget.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
-        <v>0.7024999856948853</v>
+        <v>0.7081999778747559</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - keep, try : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>The staff took the time to show me all my options, no pressure sales.</t>
+          <t>I found the perfect phone case here, and the variety was impressive.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E41" t="n">
         <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5236999988555908</v>
+        <v>0.7077999711036682</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● variety - impressive : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Amazing place to buy the latest phones at great prices!</t>
+          <t>Excellent service! They helped me find exactly what I was looking for.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1525,50 +1784,63 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F42" t="n">
-        <v>0.6916000247001648</v>
+        <v>0.7067000269889832</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - excellent : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Their warranty plan is worth every penny, such a relief!</t>
+          <t>Phone repairs took way too long, I had to come back multiple times.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-11-12</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
-        <v>0.6154999732971191</v>
+        <v>0.7039999961853027</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - have, take : Negative
+● staff - have, take : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>I appreciate how they were able to fix my phone on the same day.</t>
+          <t>Great deals on accessories, and the staff was super friendly!</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1580,73 +1852,92 @@
         <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>0.6980999708175659</v>
+        <v>0.7020000219345093</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - friendly : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Got a great deal on my new phone and an awesome case as well!</t>
+          <t>Customer service here is top-notch, they always resolve my issues quickly.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2024-11-07</t>
+          <t>2024-11-05</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E45" t="n">
         <v>2</v>
       </c>
       <c r="F45" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.7006000280380249</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - notch : Neutral
+● service - notch : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>The staff was very accommodating when I had questions about phone features.</t>
+          <t>Their warranty is useless, they refused to fix my phone under it.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2024-11-07</t>
+          <t>2024-11-12</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E46" t="n">
         <v>2</v>
       </c>
       <c r="F46" t="n">
-        <v>0.6934000253677368</v>
+        <v>0.7002999782562256</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● warranty - useless : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>I had a great experience with their trade-in program.</t>
+          <t>I appreciate how they were able to fix my phone on the same day.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2024-11-07</t>
+          <t>2024-11-06</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1655,24 +1946,30 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47" t="n">
-        <v>0.723800003528595</v>
+        <v>0.6980999708175659</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - appreciate, be : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Service was quick and efficient, I was in and out within 15 minutes!</t>
+          <t>The staff made sure I was completely comfortable with my purchase.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2024-11-07</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1684,21 +1981,27 @@
         <v>2</v>
       </c>
       <c r="F48" t="n">
-        <v>0.7379000186920166</v>
+        <v>0.6974999904632568</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - make : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>They even helped me transfer all my contacts and data without extra charge.</t>
+          <t>I love how organized the store is and how fast they attend to customers.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2024-11-08</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1710,99 +2013,123 @@
         <v>2</v>
       </c>
       <c r="F49" t="n">
-        <v>0.7339000105857849</v>
+        <v>0.6948999762535095</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - organize : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>My phone has been working flawlessly since I bought it from here.</t>
+          <t>The staff was very informative, I learned a lot about phone features I didn’t know about.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2024-11-08</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F50" t="n">
-        <v>0.680400013923645</v>
+        <v>0.6934000253677368</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - informative : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>They fixed my screen perfectly and even gave me a discount on the repair.</t>
+          <t>The staff was very accommodating when I had questions about phone features.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2024-11-08</t>
+          <t>2024-11-07</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
-        <v>0.6729000210762024</v>
+        <v>0.6934000253677368</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - accommodating : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>This is my go-to store for any phone issues, always reliable.</t>
+          <t>Very happy with the repair service here, my phone looks brand new!</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2024-11-08</t>
+          <t>2024-11-10</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F52" t="n">
-        <v>0.5602999925613403</v>
+        <v>0.682699978351593</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - look : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>They offer fantastic promotions and discounts!</t>
+          <t>They were super quick in setting up my phone, I was out of there in no time.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1814,146 +2141,184 @@
         <v>2</v>
       </c>
       <c r="F53" t="n">
-        <v>0.7225000262260437</v>
+        <v>0.6705999970436096</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - quick : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Great phone selection and even better customer service.</t>
+          <t>Very disorganized, I waited forever just to get a simple issue resolved.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54" t="n">
-        <v>0.6230999827384949</v>
+        <v>0.6575999855995178</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - wait : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>They resolved my issue very quickly and professionally.</t>
+          <t>Phone stopped working just outside the return window, terrible quality.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-16</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5146999955177307</v>
+        <v>0.633899986743927</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - stop, work : Neutral
+● phone - stop : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>I love how organized the store is and how fast they attend to customers.</t>
+          <t>Fantastic experience, the staff really know their stuff!</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E56" t="n">
         <v>2</v>
       </c>
       <c r="F56" t="n">
-        <v>0.6948999762535095</v>
+        <v>0.5684999823570251</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● experience - know : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Highly recommend this store if you’re looking for good deals on phones!</t>
+          <t>Their repair services are quick and reliable.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E57" t="n">
         <v>2</v>
       </c>
       <c r="F57" t="n">
-        <v>0.7299000024795532</v>
+        <v>0.5436999797821045</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - quick : Positive
+● service - reliable : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>I always leave this store feeling like I made the right purchase.</t>
+          <t>The staff took the time to show me all my options, no pressure sales.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-06</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E58" t="n">
         <v>2</v>
       </c>
       <c r="F58" t="n">
-        <v>0.7670999765396118</v>
+        <v>0.5236999988555908</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - take : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>I received excellent advice from the sales team, they really know their products.</t>
+          <t>Bought a phone here that stopped working within a week, very disappointing.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1963,28 +2328,34 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59" t="n">
-        <v>0.6529999971389771</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - apologetic : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Very happy with the repair service here, my phone looks brand new!</t>
+          <t>Got a great deal on my new phone and an awesome case as well!</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-07</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1996,52 +2367,64 @@
         <v>2</v>
       </c>
       <c r="F60" t="n">
-        <v>0.682699978351593</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - appreciate, be : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>I had to wait over an hour to be helped, and the staff wasn’t apologetic at all.</t>
+          <t>Upgrading my phone was a breeze thanks to their professional service.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" t="n">
-        <v>0.4941000044345856</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● variety - impressive : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Bought a phone here that stopped working within a week, very disappointing.</t>
+          <t>The phone I purchased here was overpriced compared to other stores.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2024-11-10</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E62" t="n">
@@ -2050,71 +2433,89 @@
       <c r="F62" t="n">
         <v>0.4014999866485596</v>
       </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - wait : Positive
+</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Their prices are too high, and the selection is limited.</t>
+          <t>Always come here for upgrades, they never disappoint!</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2024-11-11</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F63" t="n">
-        <v>0.7444000244140625</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - quick : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Customer service is poor, no one seemed interested in helping me.</t>
+          <t>The phone I bought here is working perfectly, couldn’t be happier.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2024-11-11</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E64" t="n">
         <v>2</v>
       </c>
       <c r="F64" t="n">
-        <v>0.7172999978065491</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - excellent : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>I had a terrible experience, the phone they sold me was defective.</t>
+          <t>Bought a refurbished phone that had several issues they didn’t disclose.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2024-11-11</t>
+          <t>2024-11-17</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2123,24 +2524,30 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F65" t="n">
-        <v>0.6730999946594238</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - feel : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>The staff was rude and unhelpful, I’m never coming back.</t>
+          <t>I’m extremely disappointed, will not be coming back here again.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2024-11-11</t>
+          <t>2024-11-17</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2152,21 +2559,28 @@
         <v>2</v>
       </c>
       <c r="F66" t="n">
-        <v>0.7110999822616577</v>
+        <v>0.4014999866485596</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● technician - damage : Neutral
+● technician - damage : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>They charged me extra for services I didn’t need, felt like a scam.</t>
+          <t>Their selection of phones is amazing, and the prices are very competitive!</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2024-11-11</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2178,73 +2592,91 @@
         <v>3</v>
       </c>
       <c r="F67" t="n">
-        <v>0.6116999983787537</v>
+        <v>0.7455000281333923</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● price - competitive : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Phone repairs took way too long, I had to come back multiple times.</t>
+          <t>Their prices are too high, and the selection is limited.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2024-11-11</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F68" t="n">
-        <v>0.7039999961853027</v>
+        <v>0.7444000244140625</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● selection - limited : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>I bought a phone, but they didn’t inform me of all the hidden fees.</t>
+          <t>The technician fixed my phone’s issue faster than I expected. Highly recommend!</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6541000008583069</v>
+        <v>0.7358999848365784</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phones issue - fix : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Staff seemed untrained and gave me incorrect information about the phone plan.</t>
+          <t>The repair was done poorly, and my phone broke again within a week.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2024-11-13</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2253,50 +2685,63 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F70" t="n">
-        <v>0.7663000226020813</v>
+        <v>0.7335000038146973</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - break : Neutral
+● phone - break : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Their warranty is useless, they refused to fix my phone under it.</t>
+          <t>I had a great experience with their trade-in program.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2024-11-07</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F71" t="n">
-        <v>0.7002999782562256</v>
+        <v>0.723800003528595</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - have : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>I had to return a faulty phone twice before they finally gave me a refund.</t>
+          <t>The technician damaged my phone during the repair, and they didn’t take responsibility.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-17</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2305,71 +2750,90 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F72" t="n">
-        <v>0.7469000220298767</v>
+        <v>0.7235999703407288</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● technician - damage : Neutral
+● technician - damage : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Very disorganized, I waited forever just to get a simple issue resolved.</t>
+          <t>I had to call multiple times just to get a response, very unprofessional.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-15</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F73" t="n">
-        <v>0.6575999855995178</v>
+        <v>0.7220000028610229</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - have, call : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>The phone I purchased here was overpriced compared to other stores.</t>
+          <t>Terrible follow-up, they lost my repair order, and I had to start over.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-17</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F74" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.7215999960899353</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - lose : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>They refused to honor the promotion I came in for, very misleading.</t>
+          <t>They didn’t even check if my phone was working after the repair.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2383,24 +2847,30 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
-        <v>0.738099992275238</v>
+        <v>0.7178999781608582</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - work : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>I felt pressured to buy accessories I didn’t need.</t>
+          <t>I love this store! Always a smooth experience buying or fixing my phone.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2409,24 +2879,30 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
-        <v>0.6230999827384949</v>
+        <v>0.7172999978065491</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● fixing - experience : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>The repair was done poorly, and my phone broke again within a week.</t>
+          <t>Terrible experience, my phone still has the same issue after getting it 'fixed'.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2438,125 +2914,160 @@
         <v>3</v>
       </c>
       <c r="F77" t="n">
-        <v>0.7335000038146973</v>
+        <v>0.7168999910354614</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - have : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Customer service was extremely slow, they need to hire more staff.</t>
+          <t>My phone was fixed in less than 30 minutes, such fast service!</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F78" t="n">
-        <v>0.4921999871730804</v>
+        <v>0.7124999761581421</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - fix : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>They didn’t even check if my phone was working after the repair.</t>
+          <t>I found exactly what I needed, and they helped me get a great deal.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2024-11-13</t>
+          <t>2024-11-04</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E79" t="n">
         <v>3</v>
       </c>
       <c r="F79" t="n">
-        <v>0.7178999781608582</v>
+        <v>0.7093999981880188</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - help, get : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Terrible experience, my phone still has the same issue after getting it 'fixed'.</t>
+          <t>I always recommend this store to friends and family, they never fail to impress.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-06</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E80" t="n">
         <v>3</v>
       </c>
       <c r="F80" t="n">
-        <v>0.7168999910354614</v>
+        <v>0.7024999856948853</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - fail, recommend : Positive
+● store - fail, recommend : Positive
+● store - fail, recommend : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>They upsold me on a phone plan I didn’t need, very deceptive.</t>
+          <t>They didn’t explain anything clearly and rushed me through the purchase.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-15</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F81" t="n">
-        <v>0.571399986743927</v>
+        <v>0.6952999830245972</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - explain : Neutral
+● store - rush : Neutral
+● store - rush : Neutral
+● store - explain : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>The staff was unprofessional and seemed like they didn’t want to be there.</t>
+          <t>The process was super simple, and I’m thrilled with my new phone.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-03</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2565,50 +3076,62 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F82" t="n">
-        <v>0.4939999878406525</v>
+        <v>0.6927000284194946</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● process - simple : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Their return policy is awful, I couldn’t exchange my phone despite its defects.</t>
+          <t>Amazing place to buy the latest phones at great prices!</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-06</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F83" t="n">
-        <v>0.7081999778747559</v>
+        <v>0.6916000247001648</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● place - amazing : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>They didn’t apply the discount I was promised.</t>
+          <t>The repair job was incomplete, and they refused to refund me.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-15</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2620,33 +3143,45 @@
         <v>3</v>
       </c>
       <c r="F84" t="n">
-        <v>0.6834999918937683</v>
+        <v>0.6915000081062317</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● job - incomplete : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>The store was messy and understaffed.</t>
+          <t>I regret buying from here, their post-purchase support is non-existent.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-15</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
-        <v>0.6488999724388123</v>
+        <v>0.6915000081062317</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● support - non : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -2674,45 +3209,57 @@
       <c r="F86" t="n">
         <v>0.6876999735832214</v>
       </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - break : Neutral
+</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>They kept trying to sell me more expensive phones when I clearly stated my budget.</t>
+          <t>Their customer service representatives were extremely rude on the phone.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2024-11-14</t>
+          <t>2024-11-15</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
-        <v>0.7081999778747559</v>
+        <v>0.6869000196456909</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● representative - rude : Negative
+</t>
+        </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>The repair job was incomplete, and they refused to refund me.</t>
+          <t>They didn’t apply the discount I was promised.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-14</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2724,47 +3271,59 @@
         <v>3</v>
       </c>
       <c r="F88" t="n">
-        <v>0.6915000081062317</v>
+        <v>0.6834999918937683</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - apply : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Their customer service representatives were extremely rude on the phone.</t>
+          <t>My phone has been working flawlessly since I bought it from here.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-08</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E89" t="n">
         <v>3</v>
       </c>
       <c r="F89" t="n">
-        <v>0.6869000196456909</v>
+        <v>0.680400013923645</v>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - work : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>I had to call multiple times just to get a response, very unprofessional.</t>
+          <t>I had a terrible experience, the phone they sold me was defective.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-11</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2776,21 +3335,27 @@
         <v>3</v>
       </c>
       <c r="F90" t="n">
-        <v>0.7220000028610229</v>
+        <v>0.6730999946594238</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● phone - defective : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>They didn’t explain anything clearly and rushed me through the purchase.</t>
+          <t>They didn’t even have the phone I wanted in stock after promising me it was available.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-16</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2802,47 +3367,62 @@
         <v>3</v>
       </c>
       <c r="F91" t="n">
-        <v>0.6952999830245972</v>
+        <v>0.6729999780654907</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - have : Positive
+● store - have : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>I regret buying from here, their post-purchase support is non-existent.</t>
+          <t>They fixed my screen perfectly and even gave me a discount on the repair.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2024-11-15</t>
+          <t>2024-11-08</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E92" t="n">
         <v>3</v>
       </c>
       <c r="F92" t="n">
-        <v>0.6915000081062317</v>
+        <v>0.6729000210762024</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - give : Neutral
+● store - fix : Positive
+● store - fix : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Phone stopped working just outside the return window, terrible quality.</t>
+          <t>Great phone selection and even better customer service.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2024-11-16</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2851,102 +3431,131 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F93" t="n">
-        <v>0.633899986743927</v>
+        <v>0.6230999827384949</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● service - great : Positive
+● service - phone : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>The store was chaotic, with long lines and unhelpful staff.</t>
+          <t>The staff were incredibly helpful and patient, helping me find the perfect phone!</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2024-11-16</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F94" t="n">
-        <v>0.6322000026702881</v>
+        <v>0.6150000095367432</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - helpful : Neutral
+● staff - patient : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>They didn’t even have the phone I wanted in stock after promising me it was available.</t>
+          <t>They charged me extra for services I didn’t need, felt like a scam.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2024-11-16</t>
+          <t>2024-11-11</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E95" t="n">
         <v>3</v>
       </c>
       <c r="F95" t="n">
-        <v>0.6729999780654907</v>
+        <v>0.6116999983787537</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● store - charge : Neutral
+● store - feel : Neutral
+● store - charge : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Terrible follow-up, they lost my repair order, and I had to start over.</t>
+          <t>I had a great experience purchasing my phone here, the process was smooth and quick.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>2024-11-17</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E96" t="n">
         <v>3</v>
       </c>
       <c r="F96" t="n">
-        <v>0.7215999960899353</v>
+        <v>0.6103000044822693</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● process - quick : Positive
+● process - smooth : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>I felt overcharged for a simple screen repair.</t>
+          <t>Staff was knowledgeable and made sure I knew everything about my new phone.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>2024-11-17</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2955,76 +3564,94 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F97" t="n">
-        <v>0.6230999827384949</v>
+        <v>0.6011000275611877</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - knowledgeable : Neutral
+</t>
+        </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Bought a refurbished phone that had several issues they didn’t disclose.</t>
+          <t>Very happy with my purchase, the staff really went the extra mile.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>2024-11-17</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F98" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.6010000109672546</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - go : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>The technician damaged my phone during the repair, and they didn’t take responsibility.</t>
+          <t>I got a really good trade-in deal on my old phone.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2024-11-17</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="E99" t="n">
         <v>3</v>
       </c>
       <c r="F99" t="n">
-        <v>0.7235999703407288</v>
+        <v>0.5996000170707703</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - get : Positive
+</t>
+        </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>I’m extremely disappointed, will not be coming back here again.</t>
+          <t>The staff was extremely helpful in setting up my phone and transferring all my data.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2024-11-17</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3033,10 +3660,16 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F100" t="n">
-        <v>0.4014999866485596</v>
+        <v>0.4796999990940094</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">● staff - helpful : Neutral
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>